<commit_message>
wrap up raw spreadsheet parsing (tests still needed)
</commit_message>
<xml_diff>
--- a/packages/spreadsheet-loaders/tests/test-wb-arango.xlsx
+++ b/packages/spreadsheet-loaders/tests/test-wb-arango.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/spreadsheet-loaders/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F99F531-1B82-2248-8E9D-84F03CD654A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAC889E-CF8F-F347-AE7E-FC96BB92EC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="3940" windowWidth="28440" windowHeight="17460" activeTab="1" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="7840" yWindow="3940" windowWidth="28440" windowHeight="17460" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name=".Date" sheetId="12" r:id="rId1"/>
-    <sheet name="BasicParsing" sheetId="1" r:id="rId2"/>
-    <sheet name=".FormulaAndRefParsing" sheetId="8" r:id="rId3"/>
-    <sheet name=".ParseErrorCases" sheetId="10" r:id="rId4"/>
-    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId5"/>
-    <sheet name=".hold" sheetId="11" r:id="rId6"/>
-    <sheet name=".lists" sheetId="7" r:id="rId7"/>
+    <sheet name="BasicParsing" sheetId="1" r:id="rId1"/>
+    <sheet name=".FormulaAndRefParsing" sheetId="8" r:id="rId2"/>
+    <sheet name=".ParseErrorCases" sheetId="10" r:id="rId3"/>
+    <sheet name=".NestedDataParsing" sheetId="9" r:id="rId4"/>
+    <sheet name=".lists" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="DataTypeList">'.lists'!$A$2:$A$8</definedName>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
   <si>
     <t>passwordHash</t>
   </si>
@@ -121,15 +119,6 @@
     <t>[1, 2, 3, 4]</t>
   </si>
   <si>
-    <t>{ a: "a", b: "b" }</t>
-  </si>
-  <si>
-    <t>{ arr: [ "a", "b", "c"] }</t>
-  </si>
-  <si>
-    <t>{ o1: { a: "a", b: "b" }}</t>
-  </si>
-  <si>
     <t>"raw string"</t>
   </si>
   <si>
@@ -193,12 +182,6 @@
     <t>uuidProp</t>
   </si>
   <si>
-    <t>uud</t>
-  </si>
-  <si>
-    <t>not-uuid</t>
-  </si>
-  <si>
     <t>refProp</t>
   </si>
   <si>
@@ -211,18 +194,12 @@
     <t>badRefProp</t>
   </si>
   <si>
-    <t>dog</t>
-  </si>
-  <si>
     <t>pw</t>
   </si>
   <si>
     <t>ariva</t>
   </si>
   <si>
-    <t>cat</t>
-  </si>
-  <si>
     <t>{ "a": 1, "b": 2 }</t>
   </si>
   <si>
@@ -233,6 +210,48 @@
   </si>
   <si>
     <t>{ "o1": {"c": "c", "d": [ "e", "f" ] }}</t>
+  </si>
+  <si>
+    <t>_auto_</t>
+  </si>
+  <si>
+    <t>invalid-uuid</t>
+  </si>
+  <si>
+    <t>f273a706-a92a-455c-be82-306744fbfbdd</t>
+  </si>
+  <si>
+    <t>skip1</t>
+  </si>
+  <si>
+    <t>skip2</t>
+  </si>
+  <si>
+    <t>don’t skip me</t>
+  </si>
+  <si>
+    <t>"don't skip"</t>
+  </si>
+  <si>
+    <t>TrUe</t>
+  </si>
+  <si>
+    <t>dont skip me</t>
+  </si>
+  <si>
+    <t>_auto_-cat</t>
+  </si>
+  <si>
+    <t>111-_auto_</t>
+  </si>
+  <si>
+    <t>black-_auto_-cat</t>
+  </si>
+  <si>
+    <t>dog-_auto_</t>
+  </si>
+  <si>
+    <t>valid6</t>
   </si>
 </sst>
 </file>
@@ -297,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,6 +343,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,85 +659,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3B61CA-6672-2444-90C9-1750BC5D5F28}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="15.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="21.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="9">
-        <v>40544</v>
-      </c>
-      <c r="F5"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{2F9FE428-81F9-4641-B514-2F573D58AE26}">
-      <formula1>WorksheetTypeList</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:G4" xr:uid="{741A365D-4032-C446-8F29-9D62D0D69A73}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:E4" xr:uid="{0DC43373-6FAB-E742-A4C9-8FB9EC7B45BB}">
-      <formula1>DataTypeList</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,7 +698,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>0</v>
@@ -759,7 +707,7 @@
         <v>16</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -776,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -785,12 +733,12 @@
         <v>9</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>-100</v>
@@ -805,18 +753,18 @@
         <v>40544</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>9999</v>
@@ -831,18 +779,18 @@
         <v>44594</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3">
         <v>9999</v>
@@ -857,18 +805,18 @@
         <v>44594</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="3">
-        <v>111</v>
+        <v>54</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>15.1515</v>
@@ -883,15 +831,18 @@
         <v>12116</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3">
         <v>-2000.1</v>
@@ -906,15 +857,18 @@
         <v>16166</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -923,7 +877,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" s="9">
         <v>20214</v>
@@ -932,49 +886,104 @@
         <v>123</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="12">
+        <v>24264</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="3" t="str">
+        <f ca="1">LOWER(CONCATENATE(DEC2HEX(RANDBETWEEN(0,4294967295),8),"-",DEC2HEX(RANDBETWEEN(0,65535),4),"-",DEC2HEX(RANDBETWEEN(16384,20479),4),"-",DEC2HEX(RANDBETWEEN(32768,49151),4),"-",DEC2HEX(RANDBETWEEN(0,65535),4),DEC2HEX(RANDBETWEEN(0,4294967295),8)))</f>
+        <v>f4177ae6-a2b7-4bd1-92f4-5117ee934419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="4" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>45</v>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:J4" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
@@ -990,7 +999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFAE23-AEC5-7049-89FE-89CD900ABF71}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1023,10 +1032,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1051,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <f>3+4*12</f>
@@ -1066,7 +1075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16853B8-B19B-5340-B113-FF91073746DD}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1095,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1114,7 +1123,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="e">
         <f>1/0</f>
@@ -1138,7 +1147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDFBAE-D0B5-F94A-A3A1-C8D39188691C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1150,168 +1159,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA8CB5D-E3AA-7F4D-B1F6-6E1C087E613F}">
-  <dimension ref="A6:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="3">
-        <v>9999</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
-        <v>44594</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="3">
-        <v>15.1515</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="9">
-        <v>12116</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="3">
-        <v>-2000.1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="9">
-        <v>16166</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="9">
-        <v>20214</v>
-      </c>
-      <c r="F9" s="3">
-        <v>123</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1350,7 +1203,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1365,7 +1218,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>